<commit_message>
add trust value on GSO
</commit_message>
<xml_diff>
--- a/selected_data.xlsx
+++ b/selected_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="245" uniqueCount="140">
   <si>
     <t>id</t>
   </si>
@@ -195,9 +195,6 @@
     <t>f_9.25</t>
   </si>
   <si>
-    <t>f_9.26</t>
-  </si>
-  <si>
     <t>route</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t>r_8</t>
   </si>
   <si>
-    <t>r_9</t>
-  </si>
-  <si>
     <t>lane</t>
   </si>
   <si>
@@ -249,9 +243,6 @@
     <t>E0_1</t>
   </si>
   <si>
-    <t>E0_0</t>
-  </si>
-  <si>
     <t>:J10_0_0</t>
   </si>
   <si>
@@ -261,9 +252,6 @@
     <t>E3_0</t>
   </si>
   <si>
-    <t>E0_1</t>
-  </si>
-  <si>
     <t>:J14_0_0</t>
   </si>
   <si>
@@ -279,9 +267,6 @@
     <t>:J0_0_0</t>
   </si>
   <si>
-    <t>E0_0</t>
-  </si>
-  <si>
     <t>-E7_0</t>
   </si>
   <si>
@@ -291,9 +276,6 @@
     <t>E5_2</t>
   </si>
   <si>
-    <t>E5_1</t>
-  </si>
-  <si>
     <t>E4_1</t>
   </si>
   <si>
@@ -306,9 +288,6 @@
     <t>-E6_1</t>
   </si>
   <si>
-    <t>-E0_0</t>
-  </si>
-  <si>
     <t>-E3_0</t>
   </si>
   <si>
@@ -318,27 +297,9 @@
     <t>:J0_1_1</t>
   </si>
   <si>
-    <t>E0_1</t>
-  </si>
-  <si>
-    <t>-E7_0</t>
-  </si>
-  <si>
-    <t>-E3_0</t>
-  </si>
-  <si>
-    <t>E3_0</t>
-  </si>
-  <si>
-    <t>E0_1</t>
-  </si>
-  <si>
     <t>E5_0</t>
   </si>
   <si>
-    <t>E4_0</t>
-  </si>
-  <si>
     <t>speed</t>
   </si>
   <si>
@@ -381,9 +342,6 @@
     <t>9.24</t>
   </si>
   <si>
-    <t>0.00</t>
-  </si>
-  <si>
     <t>4.58</t>
   </si>
   <si>
@@ -402,9 +360,6 @@
     <t>6.06</t>
   </si>
   <si>
-    <t>4.58</t>
-  </si>
-  <si>
     <t>5.01</t>
   </si>
   <si>
@@ -414,9 +369,6 @@
     <t>10.32</t>
   </si>
   <si>
-    <t>0.00</t>
-  </si>
-  <si>
     <t>1.81</t>
   </si>
   <si>
@@ -435,18 +387,12 @@
     <t>3.99</t>
   </si>
   <si>
-    <t>0.00</t>
-  </si>
-  <si>
     <t>0.25</t>
   </si>
   <si>
     <t>10.06</t>
   </si>
   <si>
-    <t>14.55</t>
-  </si>
-  <si>
     <t>14.75</t>
   </si>
   <si>
@@ -462,18 +408,9 @@
     <t>9.63</t>
   </si>
   <si>
-    <t>6.70</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
     <t>3.61</t>
   </si>
   <si>
-    <t>0.00</t>
-  </si>
-  <si>
     <t>3.84</t>
   </si>
   <si>
@@ -481,9 +418,6 @@
   </si>
   <si>
     <t>2.28</t>
-  </si>
-  <si>
-    <t>0.00</t>
   </si>
   <si>
     <t>x</t>
@@ -504,7 +438,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -543,19 +477,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.37890625" customWidth="true"/>
-    <col min="2" max="2" width="5.6015625" customWidth="true"/>
-    <col min="3" max="3" width="8.37890625" customWidth="true"/>
-    <col min="4" max="4" width="5.93359375" customWidth="true"/>
-    <col min="5" max="5" width="6.7109375" customWidth="true"/>
-    <col min="6" max="6" width="6.37890625" customWidth="true"/>
-    <col min="7" max="7" width="8.26953125" customWidth="true"/>
-    <col min="8" max="8" width="11.7109375" customWidth="true"/>
-    <col min="9" max="9" width="6.7109375" customWidth="true"/>
+    <col min="1" max="1" width="7.21875" customWidth="true"/>
+    <col min="2" max="2" width="5.44140625" customWidth="true"/>
+    <col min="3" max="3" width="8.21875" customWidth="true"/>
+    <col min="4" max="4" width="5.77734375" customWidth="true"/>
+    <col min="5" max="5" width="6.5546875" customWidth="true"/>
+    <col min="6" max="6" width="6.21875" customWidth="true"/>
+    <col min="7" max="7" width="8.109375" customWidth="true"/>
+    <col min="8" max="8" width="11.5546875" customWidth="true"/>
+    <col min="9" max="9" width="6.5546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -563,28 +500,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
@@ -592,13 +529,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E2" s="0">
         <v>244.41999999999999</v>
@@ -621,13 +558,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E3" s="0">
         <v>244.43000000000001</v>
@@ -650,13 +587,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E4" s="0">
         <v>236.93000000000001</v>
@@ -679,13 +616,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E5" s="0">
         <v>229.43000000000001</v>
@@ -708,13 +645,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E6" s="0">
         <v>221.93000000000001</v>
@@ -737,13 +674,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E7" s="0">
         <v>214.41999999999999</v>
@@ -766,13 +703,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="E8" s="0">
         <v>101.78</v>
@@ -795,13 +732,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="E9" s="0">
         <v>177.16</v>
@@ -824,13 +761,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="E10" s="0">
         <v>189.34999999999999</v>
@@ -853,13 +790,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="E11" s="0">
         <v>198.75</v>
@@ -882,13 +819,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E12" s="0">
         <v>231.13</v>
@@ -911,13 +848,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="E13" s="0">
         <v>257.99000000000001</v>
@@ -940,13 +877,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E14" s="0">
         <v>279.69</v>
@@ -969,13 +906,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="E15" s="0">
         <v>303.25999999999999</v>
@@ -998,13 +935,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="E16" s="0">
         <v>9.7799999999999994</v>
@@ -1027,13 +964,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E17" s="0">
         <v>144.21000000000001</v>
@@ -1056,13 +993,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E18" s="0">
         <v>168.44</v>
@@ -1085,13 +1022,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="E19" s="0">
         <v>252.75</v>
@@ -1114,13 +1051,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="E20" s="0">
         <v>260.57999999999998</v>
@@ -1143,13 +1080,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="E21" s="0">
         <v>260.47000000000003</v>
@@ -1172,13 +1109,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="E22" s="0">
         <v>260.11000000000001</v>
@@ -1201,13 +1138,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="E23" s="0">
         <v>95.340000000000003</v>
@@ -1230,13 +1167,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="E24" s="0">
         <v>95.75</v>
@@ -1259,13 +1196,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="E25" s="0">
         <v>97.530000000000001</v>
@@ -1288,13 +1225,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="E26" s="0">
         <v>111.81999999999999</v>
@@ -1317,13 +1254,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E27" s="0">
         <v>125.73999999999999</v>
@@ -1346,13 +1283,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="E28" s="0">
         <v>141.06</v>
@@ -1375,13 +1312,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E29" s="0">
         <v>153.78</v>
@@ -1404,13 +1341,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="E30" s="0">
         <v>167.36000000000001</v>
@@ -1433,13 +1370,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="E31" s="0">
         <v>267.69</v>
@@ -1462,13 +1399,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="E32" s="0">
         <v>254.18000000000001</v>
@@ -1491,13 +1428,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="E33" s="0">
         <v>257.38</v>
@@ -1520,13 +1457,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="E34" s="0">
         <v>254.06999999999999</v>
@@ -1549,13 +1486,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="E35" s="0">
         <v>256.89999999999998</v>
@@ -1578,13 +1515,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="E36" s="0">
         <v>261.76999999999998</v>
@@ -1607,13 +1544,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="E37" s="0">
         <v>261.25999999999999</v>
@@ -1636,13 +1573,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="E38" s="0">
         <v>261.69999999999999</v>
@@ -1665,13 +1602,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="E39" s="0">
         <v>275.93000000000001</v>
@@ -1694,13 +1631,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="E40" s="0">
         <v>327.57999999999998</v>
@@ -1723,13 +1660,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="E41" s="0">
         <v>236.91999999999999</v>
@@ -1752,13 +1689,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="E42" s="0">
         <v>229.41999999999999</v>
@@ -1781,13 +1718,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="E43" s="0">
         <v>221.91999999999999</v>
@@ -1810,13 +1747,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="E44" s="0">
         <v>214.41</v>
@@ -1839,13 +1776,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="E45" s="0">
         <v>206.81999999999999</v>
@@ -1868,13 +1805,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="E46" s="0">
         <v>2.1800000000000002</v>
@@ -1897,13 +1834,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="E47" s="0">
         <v>-26</v>
@@ -1926,13 +1863,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="E48" s="0">
         <v>6.3200000000000003</v>
@@ -1955,13 +1892,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="E49" s="0">
         <v>32.630000000000003</v>
@@ -1984,13 +1921,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="E50" s="0">
         <v>61.630000000000003</v>
@@ -2013,13 +1950,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="E51" s="0">
         <v>91.019999999999996</v>
@@ -2042,13 +1979,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="E52" s="0">
         <v>109.73999999999999</v>
@@ -2071,13 +2008,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="E53" s="0">
         <v>128.59999999999999</v>
@@ -2100,13 +2037,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>150</v>
+        <v>96</v>
       </c>
       <c r="E54" s="0">
         <v>267.37</v>
@@ -2129,13 +2066,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="E55" s="0">
         <v>268.19999999999999</v>
@@ -2158,13 +2095,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>152</v>
+        <v>96</v>
       </c>
       <c r="E56" s="0">
         <v>86.129999999999995</v>
@@ -2187,13 +2124,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="E57" s="0">
         <v>-21.079999999999998</v>
@@ -2216,13 +2153,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="E58" s="0">
         <v>28.949999999999999</v>
@@ -2245,13 +2182,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="E59" s="0">
         <v>157.66999999999999</v>
@@ -2274,13 +2211,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="E60" s="0">
         <v>250.99000000000001</v>
@@ -2296,35 +2233,6 @@
       </c>
       <c r="I60" s="0">
         <v>28.57</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="E61" s="0">
-        <v>253.69999999999999</v>
-      </c>
-      <c r="F61" s="0">
-        <v>101.29000000000001</v>
-      </c>
-      <c r="G61" s="0">
-        <v>47300</v>
-      </c>
-      <c r="H61" s="0">
-        <v>0</v>
-      </c>
-      <c r="I61" s="0">
-        <v>28.940000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>